<commit_message>
trying to plot w table 4 percent lipids in liver and muscle not getting anywhere
</commit_message>
<xml_diff>
--- a/output/Table3.xlsx
+++ b/output/Table3.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25831"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,19 +8,20 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alask\Documents\Git\cod_lipid\output\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{5E5874C2-FBB7-4DFC-8982-8EF9FE4994CA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F9A67D4-85BA-4CE7-9EF3-3DD9C14095D6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="HSI_wet_AICc" sheetId="1" r:id="rId1"/>
+    <sheet name="liverFA R results" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="35">
   <si>
     <t>df</t>
   </si>
@@ -74,14 +75,67 @@
   </si>
   <si>
     <t>Table 3.  Akaike's Information Criterion Comparisons (AICc) of various Generaized Additive Models on HSIwet.  The smaller the AICc, the better the fit.</t>
+  </si>
+  <si>
+    <t>s(J_date: year 2018)</t>
+  </si>
+  <si>
+    <t>s(J_date:year 2020)</t>
+  </si>
+  <si>
+    <t>s(TL): year 2018)</t>
+  </si>
+  <si>
+    <t>s(TL: year 2020)</t>
+  </si>
+  <si>
+    <t>sig</t>
+  </si>
+  <si>
+    <t>***</t>
+  </si>
+  <si>
+    <t>Model 5, which had the best fit, had overall R2 = 40.3, deviance explained 41.7%, GCV = 0.1615, n = 419</t>
+  </si>
+  <si>
+    <t>Model 7</t>
+  </si>
+  <si>
+    <t>year</t>
+  </si>
+  <si>
+    <t>Factor 3</t>
+  </si>
+  <si>
+    <t>Model</t>
+  </si>
+  <si>
+    <t>R2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GCV </t>
+  </si>
+  <si>
+    <t>All models have smoothing term k = 6 and sample size n = 196.  Because the percent liver fatty acids and the percent muscle fatty acids totals 100% for each fish, the model outputs are the same for percentage of muscle fatty acids</t>
+  </si>
+  <si>
+    <t>Deviance explained</t>
+  </si>
+  <si>
+    <t>Table 4.  The quasibinomial generalized additive model outputs for seven different models testing effect on the percentage of liver Fatty Acids., with smoothing term k=5 or k = 6, sample size n = 196.</t>
+  </si>
+  <si>
+    <t>Number of Iteratations to full model convergence</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <numFmts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="3">
     <numFmt numFmtId="164" formatCode="0.0"/>
+    <numFmt numFmtId="165" formatCode="0.0%"/>
+    <numFmt numFmtId="166" formatCode="0.000"/>
   </numFmts>
   <fonts count="19" x14ac:knownFonts="1">
     <font>
@@ -225,7 +279,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="33">
+  <fills count="34">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -403,6 +457,12 @@
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.39997558519241921"/>
         <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -566,16 +626,39 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="33" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -930,62 +1013,66 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F10"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:G18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
+    <col min="1" max="1" width="17.1796875" customWidth="1"/>
     <col min="2" max="2" width="4.36328125" customWidth="1"/>
     <col min="5" max="5" width="30.36328125" customWidth="1"/>
     <col min="6" max="6" width="25.54296875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A1" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="B1" s="2"/>
-      <c r="C1" s="2"/>
-      <c r="D1" s="2"/>
-      <c r="E1" s="2"/>
-      <c r="F1" s="2"/>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A2" s="2"/>
-      <c r="B2" s="2"/>
-      <c r="C2" s="2"/>
-      <c r="D2" s="2"/>
-      <c r="E2" s="2"/>
-      <c r="F2" s="2"/>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A3" s="3"/>
-      <c r="B3" s="3"/>
-      <c r="C3" s="3"/>
-      <c r="D3" s="3"/>
-      <c r="E3" s="3"/>
-      <c r="F3" s="3"/>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="B4" s="4" t="s">
+      <c r="B1" s="4"/>
+      <c r="C1" s="4"/>
+      <c r="D1" s="4"/>
+      <c r="E1" s="4"/>
+      <c r="F1" s="4"/>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A2" s="4"/>
+      <c r="B2" s="4"/>
+      <c r="C2" s="4"/>
+      <c r="D2" s="4"/>
+      <c r="E2" s="4"/>
+      <c r="F2" s="4"/>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A3" s="2"/>
+      <c r="B3" s="2"/>
+      <c r="C3" s="2"/>
+      <c r="D3" s="2"/>
+      <c r="E3" s="2"/>
+      <c r="F3" s="2"/>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="B4" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="C4" s="4" t="s">
+      <c r="C4" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="D4" s="4"/>
-      <c r="E4" s="4" t="s">
+      <c r="D4" s="3"/>
+      <c r="E4" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="F4" s="4" t="s">
+      <c r="F4" s="3" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G4" s="3" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>2</v>
       </c>
@@ -1002,7 +1089,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>3</v>
       </c>
@@ -1019,7 +1106,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>4</v>
       </c>
@@ -1033,7 +1120,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>5</v>
       </c>
@@ -1047,7 +1134,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>6</v>
       </c>
@@ -1067,21 +1154,91 @@
         <v>11</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>7</v>
       </c>
-      <c r="B10" s="1">
-        <v>5.9815027679433896</v>
-      </c>
-      <c r="C10">
-        <v>466.20706520490103</v>
-      </c>
+      <c r="B10" s="5"/>
+      <c r="C10" s="6"/>
       <c r="E10" t="s">
         <v>8</v>
       </c>
       <c r="F10" t="s">
         <v>9</v>
+      </c>
+      <c r="G10" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A11" t="s">
+        <v>25</v>
+      </c>
+      <c r="B11" s="1">
+        <v>5.9815027679433896</v>
+      </c>
+      <c r="C11">
+        <v>466.20706520490103</v>
+      </c>
+      <c r="E11" t="s">
+        <v>8</v>
+      </c>
+      <c r="F11" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A13" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="B14" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="C14" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A15" t="s">
+        <v>18</v>
+      </c>
+      <c r="B15">
+        <v>2.9449999999999998</v>
+      </c>
+      <c r="C15" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A16" t="s">
+        <v>19</v>
+      </c>
+      <c r="B16">
+        <v>3</v>
+      </c>
+      <c r="C16" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A17" t="s">
+        <v>20</v>
+      </c>
+      <c r="B17">
+        <v>1.47</v>
+      </c>
+      <c r="C17" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A18" t="s">
+        <v>21</v>
+      </c>
+      <c r="B18">
+        <v>2</v>
       </c>
     </row>
   </sheetData>
@@ -1092,4 +1249,256 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{962EECB0-DAA7-4557-86F7-3B35306A0FA7}">
+  <dimension ref="A1:I12"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F4" sqref="F4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="2" max="2" width="19.7265625" customWidth="1"/>
+    <col min="4" max="4" width="9.36328125" customWidth="1"/>
+    <col min="6" max="6" width="28.453125" customWidth="1"/>
+    <col min="7" max="7" width="28.1796875" customWidth="1"/>
+    <col min="8" max="8" width="14.54296875" customWidth="1"/>
+    <col min="9" max="9" width="27.1796875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A3" s="2"/>
+      <c r="B3" s="2"/>
+      <c r="C3" s="2"/>
+      <c r="D3" s="2"/>
+      <c r="E3" s="2"/>
+      <c r="F3" s="2"/>
+      <c r="G3" s="2"/>
+      <c r="H3" s="2"/>
+      <c r="I3" s="2"/>
+    </row>
+    <row r="4" spans="1:9" s="7" customFormat="1" ht="48" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A4" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="B4" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="C4" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="D4" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="E4" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="F4" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="G4" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="H4" s="8" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A5" s="10">
+        <v>9</v>
+      </c>
+      <c r="B5" s="10">
+        <v>5</v>
+      </c>
+      <c r="C5" s="11">
+        <v>0.4</v>
+      </c>
+      <c r="D5" s="12">
+        <v>0.45</v>
+      </c>
+      <c r="E5" s="13">
+        <v>7.1599999999999997E-2</v>
+      </c>
+      <c r="F5" t="s">
+        <v>8</v>
+      </c>
+      <c r="G5" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A6" s="10">
+        <v>10</v>
+      </c>
+      <c r="B6" s="10">
+        <v>2</v>
+      </c>
+      <c r="C6" s="11">
+        <v>0.21</v>
+      </c>
+      <c r="D6" s="12">
+        <v>0.29799999999999999</v>
+      </c>
+      <c r="E6" s="13">
+        <v>8.8499999999999995E-2</v>
+      </c>
+      <c r="F6" t="s">
+        <v>9</v>
+      </c>
+      <c r="G6" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A7" s="10">
+        <v>11</v>
+      </c>
+      <c r="B7" s="10">
+        <v>7</v>
+      </c>
+      <c r="C7" s="11">
+        <v>0.43</v>
+      </c>
+      <c r="D7" s="12">
+        <v>0.48099999999999998</v>
+      </c>
+      <c r="E7" s="13">
+        <v>7.0199999999999999E-2</v>
+      </c>
+      <c r="F7" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A8" s="10">
+        <v>12</v>
+      </c>
+      <c r="B8" s="10">
+        <v>7</v>
+      </c>
+      <c r="C8" s="11">
+        <v>0.188</v>
+      </c>
+      <c r="D8" s="12">
+        <v>0.247</v>
+      </c>
+      <c r="E8" s="13">
+        <v>9.4600000000000004E-2</v>
+      </c>
+      <c r="F8" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A9" s="10">
+        <v>13</v>
+      </c>
+      <c r="B9" s="10">
+        <v>7</v>
+      </c>
+      <c r="C9" s="11">
+        <v>0.47699999999999998</v>
+      </c>
+      <c r="D9" s="12">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="E9" s="13">
+        <v>6.2469999999999998E-2</v>
+      </c>
+      <c r="F9" t="s">
+        <v>10</v>
+      </c>
+      <c r="G9" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A10" s="10">
+        <v>14</v>
+      </c>
+      <c r="B10" s="10">
+        <v>11</v>
+      </c>
+      <c r="C10" s="11">
+        <v>0.51500000000000001</v>
+      </c>
+      <c r="D10" s="12">
+        <v>0.57999999999999996</v>
+      </c>
+      <c r="E10" s="13">
+        <v>5.9900000000000002E-2</v>
+      </c>
+      <c r="F10" t="s">
+        <v>10</v>
+      </c>
+      <c r="G10" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A11" s="10">
+        <v>15</v>
+      </c>
+      <c r="B11" s="10">
+        <v>9</v>
+      </c>
+      <c r="C11" s="11">
+        <v>0.41599999999999998</v>
+      </c>
+      <c r="D11" s="12">
+        <v>0.48399999999999999</v>
+      </c>
+      <c r="E11" s="13">
+        <v>6.6904000000000005E-2</v>
+      </c>
+      <c r="F11" t="s">
+        <v>8</v>
+      </c>
+      <c r="G11" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A12" s="10">
+        <v>16</v>
+      </c>
+      <c r="B12" s="10">
+        <v>7</v>
+      </c>
+      <c r="C12" s="11">
+        <v>0.50600000000000001</v>
+      </c>
+      <c r="D12" s="12">
+        <v>0.59099999999999997</v>
+      </c>
+      <c r="E12" s="13">
+        <v>5.62E-2</v>
+      </c>
+      <c r="F12" t="s">
+        <v>8</v>
+      </c>
+      <c r="G12" t="s">
+        <v>9</v>
+      </c>
+      <c r="H12" t="s">
+        <v>12</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
need help w blank plot space on appendix
</commit_message>
<xml_diff>
--- a/output/Table3.xlsx
+++ b/output/Table3.xlsx
@@ -1,27 +1,40 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25831"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25928"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alask\Documents\Git\cod_lipid\output\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F9A67D4-85BA-4CE7-9EF3-3DD9C14095D6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1DCDC4A9-04C7-4E1D-9839-4D87E4B74765}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="HSI_wet_AICc" sheetId="1" r:id="rId1"/>
     <sheet name="liverFA R results" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="37">
   <si>
     <t>df</t>
   </si>
@@ -62,9 +75,6 @@
     <t>Year</t>
   </si>
   <si>
-    <t>* best</t>
-  </si>
-  <si>
     <t>smoothed Total length by year</t>
   </si>
   <si>
@@ -126,6 +136,15 @@
   </si>
   <si>
     <t>Number of Iteratations to full model convergence</t>
+  </si>
+  <si>
+    <t>too much skew in data</t>
+  </si>
+  <si>
+    <t>over fit. Did not use model 16</t>
+  </si>
+  <si>
+    <t>delta</t>
   </si>
 </sst>
 </file>
@@ -626,18 +645,14 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
     <xf numFmtId="164" fontId="0" fillId="33" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -659,6 +674,11 @@
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="2" fontId="0" fillId="33" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1006,7 +1026,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme 2013 - 2022" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1016,8 +1036,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G18"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G4" sqref="G4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1029,22 +1049,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A1" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="B1" s="4"/>
-      <c r="C1" s="4"/>
-      <c r="D1" s="4"/>
-      <c r="E1" s="4"/>
-      <c r="F1" s="4"/>
+      <c r="A1" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="B1" s="12"/>
+      <c r="C1" s="12"/>
+      <c r="D1" s="12"/>
+      <c r="E1" s="12"/>
+      <c r="F1" s="12"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A2" s="4"/>
-      <c r="B2" s="4"/>
-      <c r="C2" s="4"/>
-      <c r="D2" s="4"/>
-      <c r="E2" s="4"/>
-      <c r="F2" s="4"/>
+      <c r="A2" s="12"/>
+      <c r="B2" s="12"/>
+      <c r="C2" s="12"/>
+      <c r="D2" s="12"/>
+      <c r="E2" s="12"/>
+      <c r="F2" s="12"/>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A3" s="2"/>
@@ -1061,15 +1081,17 @@
       <c r="C4" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="D4" s="3"/>
+      <c r="D4" s="3" t="s">
+        <v>36</v>
+      </c>
       <c r="E4" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="F4" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="F4" s="3" t="s">
-        <v>16</v>
-      </c>
       <c r="G4" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.35">
@@ -1079,8 +1101,12 @@
       <c r="B5" s="1">
         <v>5.9809470415795198</v>
       </c>
-      <c r="C5">
+      <c r="C5" s="13">
         <v>485.93674492276699</v>
+      </c>
+      <c r="D5" s="13">
+        <f>C5-427.58</f>
+        <v>58.356744922767007</v>
       </c>
       <c r="E5" t="s">
         <v>8</v>
@@ -1096,8 +1122,12 @@
       <c r="B6" s="1">
         <v>4.3824658281094697</v>
       </c>
-      <c r="C6">
+      <c r="C6" s="13">
         <v>579.10863409458295</v>
+      </c>
+      <c r="D6" s="13">
+        <f t="shared" ref="D6:D11" si="0">C6-427.58</f>
+        <v>151.52863409458297</v>
       </c>
       <c r="E6" t="s">
         <v>9</v>
@@ -1113,8 +1143,12 @@
       <c r="B7" s="1">
         <v>7.9229489369015003</v>
       </c>
-      <c r="C7">
+      <c r="C7" s="13">
         <v>461.50505708659603</v>
+      </c>
+      <c r="D7" s="13">
+        <f t="shared" si="0"/>
+        <v>33.925057086596041</v>
       </c>
       <c r="E7" t="s">
         <v>10</v>
@@ -1127,11 +1161,15 @@
       <c r="B8" s="1">
         <v>5.8225166230837697</v>
       </c>
-      <c r="C8">
+      <c r="C8" s="13">
         <v>581.01360098997702</v>
       </c>
+      <c r="D8" s="13">
+        <f t="shared" si="0"/>
+        <v>153.43360098997704</v>
+      </c>
       <c r="E8" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.35">
@@ -1141,11 +1179,12 @@
       <c r="B9" s="1">
         <v>11.4299752909501</v>
       </c>
-      <c r="C9">
+      <c r="C9" s="13">
         <v>427.576376449956</v>
       </c>
-      <c r="D9" t="s">
-        <v>13</v>
+      <c r="D9" s="13">
+        <f t="shared" si="0"/>
+        <v>-3.6235500439829593E-3</v>
       </c>
       <c r="E9" t="s">
         <v>10</v>
@@ -1158,8 +1197,9 @@
       <c r="A10" t="s">
         <v>7</v>
       </c>
-      <c r="B10" s="5"/>
-      <c r="C10" s="6"/>
+      <c r="B10" s="4"/>
+      <c r="C10" s="14"/>
+      <c r="D10" s="13"/>
       <c r="E10" t="s">
         <v>8</v>
       </c>
@@ -1167,18 +1207,22 @@
         <v>9</v>
       </c>
       <c r="G10" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B11" s="1">
         <v>5.9815027679433896</v>
       </c>
-      <c r="C11">
+      <c r="C11" s="13">
         <v>466.20706520490103</v>
+      </c>
+      <c r="D11" s="13">
+        <f t="shared" si="0"/>
+        <v>38.627065204901044</v>
       </c>
       <c r="E11" t="s">
         <v>8</v>
@@ -1189,7 +1233,7 @@
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.35">
@@ -1197,45 +1241,45 @@
         <v>0</v>
       </c>
       <c r="C14" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B15">
         <v>2.9449999999999998</v>
       </c>
       <c r="C15" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B16">
         <v>3</v>
       </c>
       <c r="C16" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B17">
         <v>1.47</v>
       </c>
       <c r="C17" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B18">
         <v>2</v>
@@ -1253,10 +1297,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{962EECB0-DAA7-4557-86F7-3B35306A0FA7}">
-  <dimension ref="A1:I12"/>
+  <dimension ref="A1:I13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+    <sheetView topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="H14" sqref="H14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1271,12 +1315,12 @@
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.35">
@@ -1290,46 +1334,46 @@
       <c r="H3" s="2"/>
       <c r="I3" s="2"/>
     </row>
-    <row r="4" spans="1:9" s="7" customFormat="1" ht="48" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="8" t="s">
+    <row r="4" spans="1:9" s="5" customFormat="1" ht="48" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A4" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="B4" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="C4" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="B4" s="9" t="s">
-        <v>34</v>
-      </c>
-      <c r="C4" s="8" t="s">
+      <c r="D4" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="E4" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="D4" s="9" t="s">
-        <v>32</v>
-      </c>
-      <c r="E4" s="8" t="s">
-        <v>30</v>
-      </c>
-      <c r="F4" s="8" t="s">
+      <c r="F4" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="G4" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="G4" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="H4" s="8" t="s">
-        <v>27</v>
+      <c r="H4" s="6" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A5" s="10">
+      <c r="A5" s="8">
         <v>9</v>
       </c>
-      <c r="B5" s="10">
+      <c r="B5" s="8">
         <v>5</v>
       </c>
-      <c r="C5" s="11">
+      <c r="C5" s="9">
         <v>0.4</v>
       </c>
-      <c r="D5" s="12">
+      <c r="D5" s="10">
         <v>0.45</v>
       </c>
-      <c r="E5" s="13">
+      <c r="E5" s="11">
         <v>7.1599999999999997E-2</v>
       </c>
       <c r="F5" t="s">
@@ -1340,19 +1384,19 @@
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A6" s="10">
+      <c r="A6" s="8">
         <v>10</v>
       </c>
-      <c r="B6" s="10">
+      <c r="B6" s="8">
         <v>2</v>
       </c>
-      <c r="C6" s="11">
+      <c r="C6" s="9">
         <v>0.21</v>
       </c>
-      <c r="D6" s="12">
+      <c r="D6" s="10">
         <v>0.29799999999999999</v>
       </c>
-      <c r="E6" s="13">
+      <c r="E6" s="11">
         <v>8.8499999999999995E-2</v>
       </c>
       <c r="F6" t="s">
@@ -1363,19 +1407,19 @@
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A7" s="10">
+      <c r="A7" s="8">
         <v>11</v>
       </c>
-      <c r="B7" s="10">
+      <c r="B7" s="8">
         <v>7</v>
       </c>
-      <c r="C7" s="11">
+      <c r="C7" s="9">
         <v>0.43</v>
       </c>
-      <c r="D7" s="12">
+      <c r="D7" s="10">
         <v>0.48099999999999998</v>
       </c>
-      <c r="E7" s="13">
+      <c r="E7" s="11">
         <v>7.0199999999999999E-2</v>
       </c>
       <c r="F7" t="s">
@@ -1383,39 +1427,39 @@
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A8" s="10">
+      <c r="A8" s="8">
         <v>12</v>
       </c>
-      <c r="B8" s="10">
+      <c r="B8" s="8">
         <v>7</v>
       </c>
-      <c r="C8" s="11">
+      <c r="C8" s="9">
         <v>0.188</v>
       </c>
-      <c r="D8" s="12">
+      <c r="D8" s="10">
         <v>0.247</v>
       </c>
-      <c r="E8" s="13">
+      <c r="E8" s="11">
         <v>9.4600000000000004E-2</v>
       </c>
       <c r="F8" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A9" s="10">
+      <c r="A9" s="8">
         <v>13</v>
       </c>
-      <c r="B9" s="10">
+      <c r="B9" s="8">
         <v>7</v>
       </c>
-      <c r="C9" s="11">
+      <c r="C9" s="9">
         <v>0.47699999999999998</v>
       </c>
-      <c r="D9" s="12">
+      <c r="D9" s="10">
         <v>0.55000000000000004</v>
       </c>
-      <c r="E9" s="13">
+      <c r="E9" s="11">
         <v>6.2469999999999998E-2</v>
       </c>
       <c r="F9" t="s">
@@ -1426,19 +1470,19 @@
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A10" s="10">
+      <c r="A10" s="8">
         <v>14</v>
       </c>
-      <c r="B10" s="10">
+      <c r="B10" s="8">
         <v>11</v>
       </c>
-      <c r="C10" s="11">
+      <c r="C10" s="9">
         <v>0.51500000000000001</v>
       </c>
-      <c r="D10" s="12">
+      <c r="D10" s="10">
         <v>0.57999999999999996</v>
       </c>
-      <c r="E10" s="13">
+      <c r="E10" s="11">
         <v>5.9900000000000002E-2</v>
       </c>
       <c r="F10" t="s">
@@ -1449,19 +1493,19 @@
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A11" s="10">
+      <c r="A11" s="8">
         <v>15</v>
       </c>
-      <c r="B11" s="10">
+      <c r="B11" s="8">
         <v>9</v>
       </c>
-      <c r="C11" s="11">
+      <c r="C11" s="9">
         <v>0.41599999999999998</v>
       </c>
-      <c r="D11" s="12">
+      <c r="D11" s="10">
         <v>0.48399999999999999</v>
       </c>
-      <c r="E11" s="13">
+      <c r="E11" s="11">
         <v>6.6904000000000005E-2</v>
       </c>
       <c r="F11" t="s">
@@ -1472,19 +1516,19 @@
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A12" s="10">
+      <c r="A12" s="8">
         <v>16</v>
       </c>
-      <c r="B12" s="10">
+      <c r="B12" s="8">
         <v>7</v>
       </c>
-      <c r="C12" s="11">
+      <c r="C12" s="9">
         <v>0.50600000000000001</v>
       </c>
-      <c r="D12" s="12">
+      <c r="D12" s="10">
         <v>0.59099999999999997</v>
       </c>
-      <c r="E12" s="13">
+      <c r="E12" s="11">
         <v>5.62E-2</v>
       </c>
       <c r="F12" t="s">
@@ -1495,6 +1539,14 @@
       </c>
       <c r="H12" t="s">
         <v>12</v>
+      </c>
+      <c r="I12" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="I13" t="s">
+        <v>35</v>
       </c>
     </row>
   </sheetData>

</xml_diff>